<commit_message>
Added mysql metadata compare criteria
</commit_message>
<xml_diff>
--- a/Madz.DatabaseMetaData/doc/DB_Generate_Request.xlsx
+++ b/Madz.DatabaseMetaData/doc/DB_Generate_Request.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MySQL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1242,7 +1242,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A41"/>
+      <selection activeCell="A42" sqref="A42:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>